<commit_message>
Initial version of main screen
</commit_message>
<xml_diff>
--- a/data/tag_info.xlsx
+++ b/data/tag_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Revi\Desktop\Github\Twin Shelves 2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6FC2FB-946E-4923-B616-9BE0D67E34D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04D42D3-DF37-468A-8971-336D18CE199C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{B2B09A5B-CDA6-4ED8-82F1-5DF6C662589A}"/>
+    <workbookView xWindow="4910" yWindow="3630" windowWidth="19200" windowHeight="10060" xr2:uid="{B2B09A5B-CDA6-4ED8-82F1-5DF6C662589A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C84971-4FA9-4194-B007-0AB1C52C1BED}">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="79" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -674,11 +674,11 @@
         <v>0.12722558139534884</v>
       </c>
       <c r="G2" s="4">
-        <v>35.868000000000002</v>
+        <v>37.191000000000003</v>
       </c>
       <c r="H2" s="3">
         <f>G2/D2</f>
-        <v>8.3413953488372092E-2</v>
+        <v>8.649069767441861E-2</v>
       </c>
       <c r="I2">
         <v>0.1</v>
@@ -706,11 +706,11 @@
       </c>
       <c r="G3" s="4">
         <f>G2+C2+E2</f>
-        <v>94.543999999999997</v>
+        <v>95.86699999999999</v>
       </c>
       <c r="H3" s="3">
         <f t="shared" ref="H3:H26" si="1">G3/D3</f>
-        <v>0.21986976744186046</v>
+        <v>0.22294651162790696</v>
       </c>
       <c r="I3">
         <v>0.1</v>
@@ -737,12 +737,12 @@
         <v>0.11553488372093024</v>
       </c>
       <c r="G4" s="4">
-        <f t="shared" ref="G4:G26" si="2">G3+C3+E3</f>
-        <v>203.47199999999998</v>
+        <f t="shared" ref="G4:G7" si="2">G3+C3+E3</f>
+        <v>204.79499999999999</v>
       </c>
       <c r="H4" s="3">
         <f t="shared" si="1"/>
-        <v>0.47319069767441857</v>
+        <v>0.4762674418604651</v>
       </c>
       <c r="I4">
         <v>0.1</v>
@@ -770,11 +770,11 @@
       </c>
       <c r="G5" s="4">
         <f t="shared" si="2"/>
-        <v>257.12099999999998</v>
+        <v>258.44400000000002</v>
       </c>
       <c r="H5" s="3">
         <f t="shared" si="1"/>
-        <v>0.59795581395348829</v>
+        <v>0.60103255813953493</v>
       </c>
       <c r="I5">
         <v>0.1</v>
@@ -802,11 +802,11 @@
       </c>
       <c r="G6" s="4">
         <f t="shared" si="2"/>
-        <v>290.55099999999999</v>
+        <v>291.87400000000002</v>
       </c>
       <c r="H6" s="3">
         <f t="shared" si="1"/>
-        <v>0.67569999999999997</v>
+        <v>0.67877674418604661</v>
       </c>
       <c r="I6">
         <v>0.1</v>
@@ -835,11 +835,11 @@
       </c>
       <c r="G7" s="4">
         <f t="shared" si="2"/>
-        <v>349.49899999999997</v>
+        <v>350.822</v>
       </c>
       <c r="H7" s="3">
         <f t="shared" si="1"/>
-        <v>0.81278837209302313</v>
+        <v>0.81586511627906977</v>
       </c>
       <c r="I7">
         <v>0.1</v>
@@ -866,11 +866,11 @@
         <v>0.1182906976744186</v>
       </c>
       <c r="G8">
-        <v>49.207999999999998</v>
+        <v>56.401000000000003</v>
       </c>
       <c r="H8" s="3">
         <f t="shared" si="1"/>
-        <v>0.11443720930232558</v>
+        <v>0.13116511627906977</v>
       </c>
       <c r="I8">
         <v>0.25</v>
@@ -898,11 +898,11 @@
       </c>
       <c r="G9" s="4">
         <f>G8+C8+E8</f>
-        <v>104.042</v>
+        <v>111.235</v>
       </c>
       <c r="H9" s="3">
         <f t="shared" si="1"/>
-        <v>0.24195813953488374</v>
+        <v>0.25868604651162791</v>
       </c>
       <c r="I9">
         <v>0.25</v>
@@ -930,11 +930,11 @@
       </c>
       <c r="G10" s="4">
         <f>G9+C9+E9</f>
-        <v>161.52099999999999</v>
+        <v>168.714</v>
       </c>
       <c r="H10" s="3">
         <f t="shared" si="1"/>
-        <v>0.37563023255813949</v>
+        <v>0.39235813953488374</v>
       </c>
       <c r="I10">
         <v>0.25</v>
@@ -962,11 +962,11 @@
       </c>
       <c r="G11" s="4">
         <f>G10+C10+E10</f>
-        <v>211.89299999999997</v>
+        <v>219.08599999999998</v>
       </c>
       <c r="H11" s="3">
         <f t="shared" si="1"/>
-        <v>0.4927744186046511</v>
+        <v>0.5095023255813953</v>
       </c>
       <c r="I11">
         <v>0.25</v>
@@ -994,11 +994,11 @@
       </c>
       <c r="G12" s="4">
         <f>G11+C11+E11</f>
-        <v>266.22499999999997</v>
+        <v>273.41799999999995</v>
       </c>
       <c r="H12" s="3">
         <f t="shared" si="1"/>
-        <v>0.61912790697674414</v>
+        <v>0.63585581395348822</v>
       </c>
       <c r="I12">
         <v>0.25</v>
@@ -1026,11 +1026,11 @@
       </c>
       <c r="G13" s="4">
         <f>G12+C12+E12</f>
-        <v>330.05399999999997</v>
+        <v>337.24699999999996</v>
       </c>
       <c r="H13" s="3">
         <f t="shared" si="1"/>
-        <v>0.76756744186046511</v>
+        <v>0.78429534883720919</v>
       </c>
       <c r="I13">
         <v>0.25</v>
@@ -1057,11 +1057,11 @@
         <v>0.18875581395348839</v>
       </c>
       <c r="G14">
-        <v>57.404000000000003</v>
+        <v>43.430999999999997</v>
       </c>
       <c r="H14" s="3">
         <f t="shared" si="1"/>
-        <v>0.13349767441860466</v>
+        <v>0.10100232558139534</v>
       </c>
       <c r="I14">
         <v>0.4</v>
@@ -1089,11 +1089,11 @@
       </c>
       <c r="G15" s="4">
         <f>G14+C14+E14</f>
-        <v>142.53800000000001</v>
+        <v>128.565</v>
       </c>
       <c r="H15" s="3">
         <f t="shared" si="1"/>
-        <v>0.33148372093023259</v>
+        <v>0.29898837209302326</v>
       </c>
       <c r="I15">
         <v>0.4</v>
@@ -1121,11 +1121,11 @@
       </c>
       <c r="G16" s="4">
         <f>G15+C15+E15</f>
-        <v>172.80200000000002</v>
+        <v>158.82900000000001</v>
       </c>
       <c r="H16" s="3">
         <f t="shared" si="1"/>
-        <v>0.40186511627906979</v>
+        <v>0.36936976744186051</v>
       </c>
       <c r="I16">
         <v>0.4</v>
@@ -1153,11 +1153,11 @@
       </c>
       <c r="G17" s="4">
         <f>G16+C16+E16</f>
-        <v>215.49200000000002</v>
+        <v>201.51900000000001</v>
       </c>
       <c r="H17" s="3">
         <f t="shared" si="1"/>
-        <v>0.50114418604651167</v>
+        <v>0.46864883720930234</v>
       </c>
       <c r="I17">
         <v>0.4</v>
@@ -1185,11 +1185,11 @@
       </c>
       <c r="G18" s="4">
         <f>G17+C17+E17</f>
-        <v>274.33100000000002</v>
+        <v>260.358</v>
       </c>
       <c r="H18" s="3">
         <f t="shared" si="1"/>
-        <v>0.6379790697674419</v>
+        <v>0.60548372093023262</v>
       </c>
       <c r="I18">
         <v>0.4</v>
@@ -1217,11 +1217,11 @@
       </c>
       <c r="G19" s="4">
         <f>G18+C18+E18</f>
-        <v>339.483</v>
+        <v>325.51</v>
       </c>
       <c r="H19" s="3">
         <f t="shared" si="1"/>
-        <v>0.78949534883720929</v>
+        <v>0.75700000000000001</v>
       </c>
       <c r="I19">
         <v>0.4</v>
@@ -1248,11 +1248,11 @@
         <v>0.10483720930232558</v>
       </c>
       <c r="G20">
-        <v>34.658000000000001</v>
+        <v>24.166</v>
       </c>
       <c r="H20" s="3">
         <f t="shared" si="1"/>
-        <v>8.0600000000000005E-2</v>
+        <v>5.62E-2</v>
       </c>
       <c r="I20">
         <v>0.55000000000000004</v>
@@ -1279,12 +1279,12 @@
         <v>0.12230232558139535</v>
       </c>
       <c r="G21" s="4">
-        <f>G20+C20+E20</f>
-        <v>83.706999999999994</v>
+        <f t="shared" ref="G21:G26" si="3">G20+C20+E20</f>
+        <v>73.214999999999989</v>
       </c>
       <c r="H21" s="3">
         <f t="shared" si="1"/>
-        <v>0.19466744186046511</v>
+        <v>0.17026744186046508</v>
       </c>
       <c r="I21">
         <v>0.55000000000000004</v>
@@ -1311,12 +1311,12 @@
         <v>0.12616279069767442</v>
       </c>
       <c r="G22" s="4">
-        <f>G21+C21+E21</f>
-        <v>140.26599999999999</v>
+        <f t="shared" si="3"/>
+        <v>129.774</v>
       </c>
       <c r="H22" s="3">
         <f t="shared" si="1"/>
-        <v>0.32619999999999999</v>
+        <v>0.30180000000000001</v>
       </c>
       <c r="I22">
         <v>0.55000000000000004</v>
@@ -1343,12 +1343,12 @@
         <v>0.13619767441860464</v>
       </c>
       <c r="G23" s="4">
-        <f>G22+C22+E22</f>
-        <v>198.48499999999999</v>
+        <f t="shared" si="3"/>
+        <v>187.99299999999999</v>
       </c>
       <c r="H23" s="3">
         <f t="shared" si="1"/>
-        <v>0.46159302325581392</v>
+        <v>0.43719302325581394</v>
       </c>
       <c r="I23">
         <v>0.55000000000000004</v>
@@ -1375,12 +1375,12 @@
         <v>0.13369767441860467</v>
       </c>
       <c r="G24" s="4">
-        <f>G23+C23+E23</f>
-        <v>261.01899999999995</v>
+        <f t="shared" si="3"/>
+        <v>250.52699999999999</v>
       </c>
       <c r="H24" s="3">
         <f t="shared" si="1"/>
-        <v>0.60702093023255799</v>
+        <v>0.58262093023255812</v>
       </c>
       <c r="I24">
         <v>0.55000000000000004</v>
@@ -1407,12 +1407,12 @@
         <v>0.10604651162790699</v>
       </c>
       <c r="G25" s="4">
-        <f>G24+C24+E24</f>
-        <v>322.47799999999995</v>
+        <f t="shared" si="3"/>
+        <v>311.98599999999999</v>
       </c>
       <c r="H25" s="3">
         <f t="shared" si="1"/>
-        <v>0.74994883720930217</v>
+        <v>0.7255488372093023</v>
       </c>
       <c r="I25">
         <v>0.55000000000000004</v>
@@ -1439,12 +1439,12 @@
         <v>0.10296976744186047</v>
       </c>
       <c r="G26" s="4">
-        <f>G25+C25+E25</f>
-        <v>372.04699999999997</v>
+        <f t="shared" si="3"/>
+        <v>361.55500000000001</v>
       </c>
       <c r="H26" s="3">
         <f t="shared" si="1"/>
-        <v>0.86522558139534878</v>
+        <v>0.8408255813953488</v>
       </c>
       <c r="I26">
         <v>0.55000000000000004</v>

</xml_diff>

<commit_message>
Added text on top of magnifying glass
</commit_message>
<xml_diff>
--- a/data/tag_info.xlsx
+++ b/data/tag_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Revi\Desktop\Github\Twin Shelves 2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04D42D3-DF37-468A-8971-336D18CE199C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6DFC7F-2489-4CFD-A4F5-873D2A111150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4910" yWindow="3630" windowWidth="19200" windowHeight="10060" xr2:uid="{B2B09A5B-CDA6-4ED8-82F1-5DF6C662589A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{B2B09A5B-CDA6-4ED8-82F1-5DF6C662589A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>topic_1</t>
   </si>
@@ -216,17 +216,27 @@
   </si>
   <si>
     <t>start_y_percentage</t>
+  </si>
+  <si>
+    <t>tag_height</t>
+  </si>
+  <si>
+    <t>row</t>
+  </si>
+  <si>
+    <t>spacer_height</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,6 +246,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -258,10 +276,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -273,8 +292,15 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -607,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C84971-4FA9-4194-B007-0AB1C52C1BED}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="79" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
+      <selection activeCell="I26" sqref="A1:I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -618,13 +644,14 @@
     <col min="1" max="1" width="36.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.81640625" customWidth="1"/>
     <col min="4" max="4" width="10.81640625" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.1796875" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1796875" customWidth="1"/>
+    <col min="8" max="8" width="3.90625" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -638,22 +665,28 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
         <v>12</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="I1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="N1" t="s">
+        <v>60</v>
+      </c>
+      <c r="O1">
+        <v>8.5180000000000007</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -661,30 +694,37 @@
         <v>0</v>
       </c>
       <c r="C2" s="4">
-        <v>54.707000000000001</v>
+        <v>44.38</v>
       </c>
       <c r="D2" s="1">
         <v>430</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
+        <f>C2/D2</f>
+        <v>0.1032093023255814</v>
+      </c>
+      <c r="F2" s="4">
+        <v>70.754999999999995</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2/D2</f>
+        <v>0.16454651162790696</v>
+      </c>
+      <c r="H2" s="5">
+        <v>1</v>
+      </c>
+      <c r="I2" s="7">
+        <f>(3+(H2-1)*($O$1+$O$3))/(48.732+5)</f>
+        <v>5.5832650934266356E-2</v>
+      </c>
+      <c r="N2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2">
         <v>3.9689999999999999</v>
       </c>
-      <c r="F2" s="3">
-        <f>C2/D2</f>
-        <v>0.12722558139534884</v>
-      </c>
-      <c r="G2" s="4">
-        <v>37.191000000000003</v>
-      </c>
-      <c r="H2" s="3">
-        <f>G2/D2</f>
-        <v>8.649069767441861E-2</v>
-      </c>
-      <c r="I2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -692,31 +732,38 @@
         <v>1</v>
       </c>
       <c r="C3" s="4">
-        <v>104.959</v>
+        <v>85.145967060888012</v>
       </c>
       <c r="D3" s="1">
         <v>430</v>
       </c>
-      <c r="E3" s="4">
-        <v>3.9689999999999999</v>
-      </c>
-      <c r="F3" s="3">
-        <f t="shared" ref="F3:F26" si="0">C3/D3</f>
-        <v>0.2440906976744186</v>
-      </c>
-      <c r="G3" s="4">
-        <f>G2+C2+E2</f>
-        <v>95.86699999999999</v>
-      </c>
-      <c r="H3" s="3">
-        <f t="shared" ref="H3:H26" si="1">G3/D3</f>
-        <v>0.22294651162790696</v>
-      </c>
-      <c r="I3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E3" s="3">
+        <f>C3/D3</f>
+        <v>0.19801387688578606</v>
+      </c>
+      <c r="F3" s="4">
+        <f>F2+C2+$O$2</f>
+        <v>119.10399999999998</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3/D3</f>
+        <v>0.27698604651162789</v>
+      </c>
+      <c r="H3" s="5">
+        <v>1</v>
+      </c>
+      <c r="I3" s="7">
+        <f t="shared" ref="I3:I26" si="0">(3+(H3-1)*($O$1+$O$3))/(48.732+5)</f>
+        <v>5.5832650934266356E-2</v>
+      </c>
+      <c r="N3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -724,31 +771,32 @@
         <v>2</v>
       </c>
       <c r="C4" s="4">
-        <v>49.68</v>
+        <v>40.301943078582269</v>
       </c>
       <c r="D4" s="1">
         <v>430</v>
       </c>
-      <c r="E4" s="4">
-        <v>3.9689999999999999</v>
-      </c>
-      <c r="F4" s="3">
-        <f t="shared" si="0"/>
-        <v>0.11553488372093024</v>
-      </c>
-      <c r="G4" s="4">
-        <f t="shared" ref="G4:G7" si="2">G3+C3+E3</f>
-        <v>204.79499999999999</v>
-      </c>
-      <c r="H4" s="3">
-        <f t="shared" si="1"/>
-        <v>0.4762674418604651</v>
-      </c>
-      <c r="I4">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E4" s="3">
+        <f>C4/D4</f>
+        <v>9.3725449019958759E-2</v>
+      </c>
+      <c r="F4" s="4">
+        <f>F3+C3+$O$2</f>
+        <v>208.21896706088799</v>
+      </c>
+      <c r="G4" s="3">
+        <f>F4/D4</f>
+        <v>0.48423015595555347</v>
+      </c>
+      <c r="H4" s="5">
+        <v>1</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="0"/>
+        <v>5.5832650934266356E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -756,31 +804,32 @@
         <v>3</v>
       </c>
       <c r="C5" s="4">
-        <v>29.460999999999999</v>
+        <v>23.89966878096039</v>
       </c>
       <c r="D5" s="1">
         <v>430</v>
       </c>
-      <c r="E5" s="4">
-        <v>3.9689999999999999</v>
-      </c>
-      <c r="F5" s="3">
-        <f t="shared" si="0"/>
-        <v>6.8513953488372095E-2</v>
-      </c>
-      <c r="G5" s="4">
-        <f t="shared" si="2"/>
-        <v>258.44400000000002</v>
-      </c>
-      <c r="H5" s="3">
-        <f t="shared" si="1"/>
-        <v>0.60103255813953493</v>
-      </c>
-      <c r="I5">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E5" s="3">
+        <f>C5/D5</f>
+        <v>5.5580625072000907E-2</v>
+      </c>
+      <c r="F5" s="4">
+        <f>F4+C4+$O$2</f>
+        <v>252.48991013947025</v>
+      </c>
+      <c r="G5" s="3">
+        <f>F5/D5</f>
+        <v>0.58718583753365172</v>
+      </c>
+      <c r="H5" s="5">
+        <v>1</v>
+      </c>
+      <c r="I5" s="7">
+        <f t="shared" si="0"/>
+        <v>5.5832650934266356E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -788,32 +837,33 @@
         <v>4</v>
       </c>
       <c r="C6" s="4">
-        <v>54.978999999999999</v>
+        <v>44.600654760816717</v>
       </c>
       <c r="D6" s="1">
         <v>430</v>
       </c>
-      <c r="E6" s="4">
-        <v>3.9689999999999999</v>
-      </c>
-      <c r="F6" s="3">
-        <f t="shared" si="0"/>
-        <v>0.12785813953488373</v>
-      </c>
-      <c r="G6" s="4">
-        <f t="shared" si="2"/>
-        <v>291.87400000000002</v>
-      </c>
-      <c r="H6" s="3">
-        <f t="shared" si="1"/>
-        <v>0.67877674418604661</v>
-      </c>
-      <c r="I6">
-        <v>0.1</v>
+      <c r="E6" s="3">
+        <f>C6/D6</f>
+        <v>0.10372245293213191</v>
+      </c>
+      <c r="F6" s="4">
+        <f>F5+C5+$O$2</f>
+        <v>280.35857892043066</v>
+      </c>
+      <c r="G6" s="3">
+        <f>F6/D6</f>
+        <v>0.65199669516379222</v>
+      </c>
+      <c r="H6" s="5">
+        <v>1</v>
+      </c>
+      <c r="I6" s="7">
+        <f t="shared" si="0"/>
+        <v>5.5832650934266356E-2</v>
       </c>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -821,314 +871,324 @@
         <v>5</v>
       </c>
       <c r="C7" s="4">
-        <v>41.988</v>
+        <v>34.06195623960371</v>
       </c>
       <c r="D7" s="1">
         <v>430</v>
       </c>
-      <c r="E7" s="4">
-        <v>3.9689999999999999</v>
-      </c>
-      <c r="F7" s="3">
-        <f t="shared" si="0"/>
-        <v>9.7646511627906982E-2</v>
-      </c>
-      <c r="G7" s="4">
-        <f t="shared" si="2"/>
-        <v>350.822</v>
-      </c>
-      <c r="H7" s="3">
-        <f t="shared" si="1"/>
-        <v>0.81586511627906977</v>
-      </c>
-      <c r="I7">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E7" s="3">
+        <f>C7/D7</f>
+        <v>7.9213851720008624E-2</v>
+      </c>
+      <c r="F7" s="4">
+        <f>F6+C6+$O$2</f>
+        <v>328.92823368124738</v>
+      </c>
+      <c r="G7" s="3">
+        <f>F7/D7</f>
+        <v>0.7649493806540637</v>
+      </c>
+      <c r="H7" s="5">
+        <v>1</v>
+      </c>
+      <c r="I7" s="7">
+        <f t="shared" si="0"/>
+        <v>5.5832650934266356E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>21</v>
       </c>
       <c r="B8" t="s">
         <v>40</v>
       </c>
-      <c r="C8">
-        <v>50.865000000000002</v>
+      <c r="C8" s="4">
+        <v>41.263251503463913</v>
       </c>
       <c r="D8" s="1">
         <v>430</v>
       </c>
-      <c r="E8" s="4">
-        <v>3.9689999999999999</v>
-      </c>
-      <c r="F8" s="3">
-        <f t="shared" si="0"/>
-        <v>0.1182906976744186</v>
-      </c>
-      <c r="G8">
-        <v>56.401000000000003</v>
-      </c>
-      <c r="H8" s="3">
-        <f t="shared" si="1"/>
-        <v>0.13116511627906977</v>
-      </c>
-      <c r="I8">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E8" s="3">
+        <f>C8/D8</f>
+        <v>9.5961050008055618E-2</v>
+      </c>
+      <c r="F8">
+        <v>86.338999999999999</v>
+      </c>
+      <c r="G8" s="3">
+        <f>F8/D8</f>
+        <v>0.20078837209302325</v>
+      </c>
+      <c r="H8" s="5">
+        <v>2</v>
+      </c>
+      <c r="I8" s="7">
+        <f t="shared" si="0"/>
+        <v>0.23297104146504877</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>22</v>
       </c>
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9">
-        <v>53.51</v>
+      <c r="C9" s="4">
+        <v>43.4089568062588</v>
       </c>
       <c r="D9" s="1">
         <v>430</v>
       </c>
-      <c r="E9" s="4">
-        <v>3.9689999999999999</v>
-      </c>
-      <c r="F9" s="3">
-        <f t="shared" si="0"/>
-        <v>0.12444186046511628</v>
-      </c>
-      <c r="G9" s="4">
-        <f>G8+C8+E8</f>
-        <v>111.235</v>
-      </c>
-      <c r="H9" s="3">
-        <f t="shared" si="1"/>
-        <v>0.25868604651162791</v>
-      </c>
-      <c r="I9">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E9" s="3">
+        <f>C9/D9</f>
+        <v>0.10095106234013675</v>
+      </c>
+      <c r="F9" s="4">
+        <f>F8+C8+$O$2</f>
+        <v>131.57125150346391</v>
+      </c>
+      <c r="G9" s="3">
+        <f>F9/D9</f>
+        <v>0.30597965465921839</v>
+      </c>
+      <c r="H9" s="5">
+        <v>2</v>
+      </c>
+      <c r="I9" s="7">
+        <f t="shared" si="0"/>
+        <v>0.23297104146504877</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>23</v>
       </c>
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10">
-        <v>46.402999999999999</v>
+      <c r="C10" s="4">
+        <v>37.643539949183833</v>
       </c>
       <c r="D10" s="1">
         <v>430</v>
       </c>
-      <c r="E10" s="4">
-        <v>3.9689999999999999</v>
-      </c>
-      <c r="F10" s="3">
-        <f t="shared" si="0"/>
-        <v>0.10791395348837209</v>
-      </c>
-      <c r="G10" s="4">
-        <f>G9+C9+E9</f>
-        <v>168.714</v>
-      </c>
-      <c r="H10" s="3">
-        <f t="shared" si="1"/>
-        <v>0.39235813953488374</v>
-      </c>
-      <c r="I10">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E10" s="3">
+        <f>C10/D10</f>
+        <v>8.7543116160892637E-2</v>
+      </c>
+      <c r="F10" s="4">
+        <f t="shared" ref="F10:F13" si="1">F9+C9+$O$2</f>
+        <v>178.94920830972271</v>
+      </c>
+      <c r="G10" s="3">
+        <f>F10/D10</f>
+        <v>0.41616094955749466</v>
+      </c>
+      <c r="H10" s="5">
+        <v>2</v>
+      </c>
+      <c r="I10" s="7">
+        <f t="shared" si="0"/>
+        <v>0.23297104146504877</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="C11">
-        <v>50.363</v>
+      <c r="C11" s="4">
+        <v>40.856013672838941</v>
       </c>
       <c r="D11" s="1">
         <v>430</v>
       </c>
-      <c r="E11" s="4">
-        <v>3.9689999999999999</v>
-      </c>
-      <c r="F11" s="3">
-        <f t="shared" si="0"/>
-        <v>0.11712325581395348</v>
-      </c>
-      <c r="G11" s="4">
-        <f>G10+C10+E10</f>
-        <v>219.08599999999998</v>
-      </c>
-      <c r="H11" s="3">
+      <c r="E11" s="3">
+        <f>C11/D11</f>
+        <v>9.5013985285671954E-2</v>
+      </c>
+      <c r="F11" s="4">
         <f t="shared" si="1"/>
-        <v>0.5095023255813953</v>
-      </c>
-      <c r="I11">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+        <v>220.56174825890653</v>
+      </c>
+      <c r="G11" s="3">
+        <f>F11/D11</f>
+        <v>0.51293429827652681</v>
+      </c>
+      <c r="H11" s="5">
+        <v>2</v>
+      </c>
+      <c r="I11" s="7">
+        <f t="shared" si="0"/>
+        <v>0.23297104146504877</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>25</v>
       </c>
       <c r="B12" t="s">
         <v>44</v>
       </c>
-      <c r="C12">
-        <v>59.86</v>
+      <c r="C12" s="4">
+        <v>48.560271994443127</v>
       </c>
       <c r="D12" s="1">
         <v>430</v>
       </c>
-      <c r="E12" s="4">
-        <v>3.9689999999999999</v>
-      </c>
-      <c r="F12" s="3">
-        <f t="shared" si="0"/>
-        <v>0.1392093023255814</v>
-      </c>
-      <c r="G12" s="4">
-        <f>G11+C11+E11</f>
-        <v>273.41799999999995</v>
-      </c>
-      <c r="H12" s="3">
+      <c r="E12" s="3">
+        <f>C12/D12</f>
+        <v>0.11293086510335611</v>
+      </c>
+      <c r="F12" s="4">
         <f t="shared" si="1"/>
-        <v>0.63585581395348822</v>
-      </c>
-      <c r="I12">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+        <v>265.38676193174547</v>
+      </c>
+      <c r="G12" s="3">
+        <f>F12/D12</f>
+        <v>0.61717851612033825</v>
+      </c>
+      <c r="H12" s="5">
+        <v>2</v>
+      </c>
+      <c r="I12" s="7">
+        <f t="shared" si="0"/>
+        <v>0.23297104146504877</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>26</v>
       </c>
       <c r="B13" t="s">
         <v>45</v>
       </c>
-      <c r="C13">
-        <v>36.348999999999997</v>
+      <c r="C13" s="4">
+        <v>29.487426106348362</v>
       </c>
       <c r="D13" s="1">
         <v>430</v>
       </c>
-      <c r="E13" s="4">
-        <v>3.9689999999999999</v>
-      </c>
-      <c r="F13" s="3">
-        <f t="shared" si="0"/>
-        <v>8.4532558139534877E-2</v>
-      </c>
-      <c r="G13" s="4">
-        <f>G12+C12+E12</f>
-        <v>337.24699999999996</v>
-      </c>
-      <c r="H13" s="3">
+      <c r="E13" s="3">
+        <f>C13/D13</f>
+        <v>6.8575409549647359E-2</v>
+      </c>
+      <c r="F13" s="4">
         <f t="shared" si="1"/>
-        <v>0.78429534883720919</v>
-      </c>
-      <c r="I13">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+        <v>317.91603392618862</v>
+      </c>
+      <c r="G13" s="3">
+        <f>F13/D13</f>
+        <v>0.73933961378183399</v>
+      </c>
+      <c r="H13" s="5">
+        <v>2</v>
+      </c>
+      <c r="I13" s="7">
+        <f t="shared" si="0"/>
+        <v>0.23297104146504877</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>27</v>
       </c>
       <c r="B14" t="s">
         <v>46</v>
       </c>
-      <c r="C14">
-        <v>81.165000000000006</v>
+      <c r="C14" s="4">
+        <v>65.84354287385527</v>
       </c>
       <c r="D14" s="1">
         <v>430</v>
       </c>
-      <c r="E14" s="4">
-        <v>3.9689999999999999</v>
-      </c>
-      <c r="F14" s="3">
-        <f t="shared" si="0"/>
-        <v>0.18875581395348839</v>
-      </c>
-      <c r="G14">
-        <v>43.430999999999997</v>
-      </c>
-      <c r="H14" s="3">
-        <f t="shared" si="1"/>
-        <v>0.10100232558139534</v>
-      </c>
-      <c r="I14">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E14" s="3">
+        <f>C14/D14</f>
+        <v>0.15312451831129131</v>
+      </c>
+      <c r="F14">
+        <v>75.816999999999993</v>
+      </c>
+      <c r="G14" s="3">
+        <f>F14/D14</f>
+        <v>0.17631860465116278</v>
+      </c>
+      <c r="H14" s="5">
+        <v>3</v>
+      </c>
+      <c r="I14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.41010943199583122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>28</v>
       </c>
       <c r="B15" t="s">
         <v>47</v>
       </c>
-      <c r="C15">
-        <v>26.295000000000002</v>
+      <c r="C15" s="4">
+        <v>21.331312263512899</v>
       </c>
       <c r="D15" s="1">
         <v>430</v>
       </c>
-      <c r="E15" s="4">
-        <v>3.9689999999999999</v>
-      </c>
-      <c r="F15" s="3">
-        <f t="shared" si="0"/>
-        <v>6.1151162790697676E-2</v>
-      </c>
-      <c r="G15" s="4">
-        <f>G14+C14+E14</f>
-        <v>128.565</v>
-      </c>
-      <c r="H15" s="3">
-        <f t="shared" si="1"/>
-        <v>0.29898837209302326</v>
-      </c>
-      <c r="I15">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E15" s="3">
+        <f>C15/D15</f>
+        <v>4.9607702938402089E-2</v>
+      </c>
+      <c r="F15" s="4">
+        <f>F14+C14+$O$2</f>
+        <v>145.62954287385526</v>
+      </c>
+      <c r="G15" s="3">
+        <f>F15/D15</f>
+        <v>0.33867335552059363</v>
+      </c>
+      <c r="H15" s="5">
+        <v>3</v>
+      </c>
+      <c r="I15" s="7">
+        <f t="shared" si="0"/>
+        <v>0.41010943199583122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>29</v>
       </c>
       <c r="B16" t="s">
         <v>48</v>
       </c>
-      <c r="C16">
-        <v>38.720999999999997</v>
+      <c r="C16" s="4">
+        <v>31.411665417588242</v>
       </c>
       <c r="D16" s="1">
         <v>430</v>
       </c>
-      <c r="E16" s="4">
-        <v>3.9689999999999999</v>
-      </c>
-      <c r="F16" s="3">
-        <f t="shared" si="0"/>
-        <v>9.0048837209302318E-2</v>
-      </c>
-      <c r="G16" s="4">
-        <f>G15+C15+E15</f>
-        <v>158.82900000000001</v>
-      </c>
-      <c r="H16" s="3">
-        <f t="shared" si="1"/>
-        <v>0.36936976744186051</v>
-      </c>
-      <c r="I16">
-        <v>0.4</v>
+      <c r="E16" s="3">
+        <f>C16/D16</f>
+        <v>7.3050384692065679E-2</v>
+      </c>
+      <c r="F16" s="4">
+        <f t="shared" ref="F16:F19" si="2">F15+C15+$O$2</f>
+        <v>170.92985513736815</v>
+      </c>
+      <c r="G16" s="3">
+        <f>F16/D16</f>
+        <v>0.39751129101713523</v>
+      </c>
+      <c r="H16" s="5">
+        <v>3</v>
+      </c>
+      <c r="I16" s="7">
+        <f t="shared" si="0"/>
+        <v>0.41010943199583122</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -1138,29 +1198,30 @@
       <c r="B17" t="s">
         <v>49</v>
       </c>
-      <c r="C17">
-        <v>54.87</v>
+      <c r="C17" s="4">
+        <v>44.512230610342371</v>
       </c>
       <c r="D17" s="1">
         <v>430</v>
       </c>
-      <c r="E17" s="4">
-        <v>3.9689999999999999</v>
-      </c>
-      <c r="F17" s="3">
-        <f t="shared" si="0"/>
-        <v>0.12760465116279068</v>
-      </c>
-      <c r="G17" s="4">
-        <f>G16+C16+E16</f>
-        <v>201.51900000000001</v>
-      </c>
-      <c r="H17" s="3">
-        <f t="shared" si="1"/>
-        <v>0.46864883720930234</v>
-      </c>
-      <c r="I17">
-        <v>0.4</v>
+      <c r="E17" s="3">
+        <f>C17/D17</f>
+        <v>0.10351681537288923</v>
+      </c>
+      <c r="F17" s="4">
+        <f t="shared" si="2"/>
+        <v>206.31052055495638</v>
+      </c>
+      <c r="G17" s="3">
+        <f>F17/D17</f>
+        <v>0.47979190826734042</v>
+      </c>
+      <c r="H17" s="5">
+        <v>3</v>
+      </c>
+      <c r="I17" s="7">
+        <f t="shared" si="0"/>
+        <v>0.41010943199583122</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -1170,29 +1231,30 @@
       <c r="B18" t="s">
         <v>50</v>
       </c>
-      <c r="C18">
-        <v>61.183</v>
+      <c r="C18" s="4">
+        <v>49.633530261209721</v>
       </c>
       <c r="D18" s="1">
         <v>430</v>
       </c>
-      <c r="E18" s="4">
-        <v>3.9689999999999999</v>
-      </c>
-      <c r="F18" s="3">
-        <f t="shared" si="0"/>
-        <v>0.14228604651162791</v>
-      </c>
-      <c r="G18" s="4">
-        <f>G17+C17+E17</f>
-        <v>260.358</v>
-      </c>
-      <c r="H18" s="3">
-        <f t="shared" si="1"/>
-        <v>0.60548372093023262</v>
-      </c>
-      <c r="I18">
-        <v>0.4</v>
+      <c r="E18" s="3">
+        <f>C18/D18</f>
+        <v>0.11542681456095284</v>
+      </c>
+      <c r="F18" s="4">
+        <f t="shared" si="2"/>
+        <v>254.79175116529876</v>
+      </c>
+      <c r="G18" s="3">
+        <f>F18/D18</f>
+        <v>0.59253895619836927</v>
+      </c>
+      <c r="H18" s="5">
+        <v>3</v>
+      </c>
+      <c r="I18" s="7">
+        <f t="shared" si="0"/>
+        <v>0.41010943199583122</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -1202,29 +1264,30 @@
       <c r="B19" t="s">
         <v>51</v>
       </c>
-      <c r="C19">
-        <v>61.057000000000002</v>
+      <c r="C19" s="4">
+        <v>49.53131518818433</v>
       </c>
       <c r="D19" s="1">
         <v>430</v>
       </c>
-      <c r="E19" s="4">
-        <v>3.9689999999999999</v>
-      </c>
-      <c r="F19" s="3">
-        <f t="shared" si="0"/>
-        <v>0.14199302325581395</v>
-      </c>
-      <c r="G19" s="4">
-        <f>G18+C18+E18</f>
-        <v>325.51</v>
-      </c>
-      <c r="H19" s="3">
-        <f t="shared" si="1"/>
-        <v>0.75700000000000001</v>
-      </c>
-      <c r="I19">
-        <v>0.4</v>
+      <c r="E19" s="3">
+        <f>C19/D19</f>
+        <v>0.11518910508880077</v>
+      </c>
+      <c r="F19" s="4">
+        <f t="shared" si="2"/>
+        <v>308.39428142650848</v>
+      </c>
+      <c r="G19" s="3">
+        <f>F19/D19</f>
+        <v>0.71719600331746158</v>
+      </c>
+      <c r="H19" s="5">
+        <v>3</v>
+      </c>
+      <c r="I19" s="7">
+        <f t="shared" si="0"/>
+        <v>0.41010943199583122</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -1234,28 +1297,29 @@
       <c r="B20" t="s">
         <v>52</v>
       </c>
-      <c r="C20">
-        <v>45.08</v>
+      <c r="C20" s="4">
+        <v>36.570281682417239</v>
       </c>
       <c r="D20" s="1">
         <v>430</v>
       </c>
-      <c r="E20" s="4">
-        <v>3.9689999999999999</v>
-      </c>
-      <c r="F20" s="3">
-        <f t="shared" si="0"/>
-        <v>0.10483720930232558</v>
-      </c>
-      <c r="G20">
-        <v>24.166</v>
-      </c>
-      <c r="H20" s="3">
-        <f t="shared" si="1"/>
-        <v>5.62E-2</v>
-      </c>
-      <c r="I20">
-        <v>0.55000000000000004</v>
+      <c r="E20" s="3">
+        <f>C20/D20</f>
+        <v>8.5047166703295901E-2</v>
+      </c>
+      <c r="F20">
+        <v>60.189</v>
+      </c>
+      <c r="G20" s="3">
+        <f>F20/D20</f>
+        <v>0.13997441860465115</v>
+      </c>
+      <c r="H20" s="5">
+        <v>4</v>
+      </c>
+      <c r="I20" s="7">
+        <f t="shared" si="0"/>
+        <v>0.58724782252661356</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -1265,29 +1329,30 @@
       <c r="B21" t="s">
         <v>53</v>
       </c>
-      <c r="C21">
-        <v>52.59</v>
+      <c r="C21" s="4">
+        <v>42.662624527025798</v>
       </c>
       <c r="D21" s="1">
         <v>430</v>
       </c>
-      <c r="E21" s="4">
-        <v>3.9689999999999999</v>
-      </c>
-      <c r="F21" s="3">
-        <f t="shared" si="0"/>
-        <v>0.12230232558139535</v>
-      </c>
-      <c r="G21" s="4">
-        <f t="shared" ref="G21:G26" si="3">G20+C20+E20</f>
-        <v>73.214999999999989</v>
-      </c>
-      <c r="H21" s="3">
-        <f t="shared" si="1"/>
-        <v>0.17026744186046508</v>
-      </c>
-      <c r="I21">
-        <v>0.55000000000000004</v>
+      <c r="E21" s="3">
+        <f>C21/D21</f>
+        <v>9.9215405876804177E-2</v>
+      </c>
+      <c r="F21" s="4">
+        <f>F20+C20+$O$2</f>
+        <v>100.72828168241723</v>
+      </c>
+      <c r="G21" s="3">
+        <f>F21/D21</f>
+        <v>0.23425181786608659</v>
+      </c>
+      <c r="H21" s="5">
+        <v>4</v>
+      </c>
+      <c r="I21" s="7">
+        <f t="shared" si="0"/>
+        <v>0.58724782252661356</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -1297,29 +1362,30 @@
       <c r="B22" t="s">
         <v>54</v>
       </c>
-      <c r="C22">
-        <v>54.25</v>
+      <c r="C22" s="4">
+        <v>44.009267552598388</v>
       </c>
       <c r="D22" s="1">
         <v>430</v>
       </c>
-      <c r="E22" s="4">
-        <v>3.9689999999999999</v>
-      </c>
-      <c r="F22" s="3">
-        <f t="shared" si="0"/>
-        <v>0.12616279069767442</v>
-      </c>
-      <c r="G22" s="4">
-        <f t="shared" si="3"/>
-        <v>129.774</v>
-      </c>
-      <c r="H22" s="3">
-        <f t="shared" si="1"/>
-        <v>0.30180000000000001</v>
-      </c>
-      <c r="I22">
-        <v>0.55000000000000004</v>
+      <c r="E22" s="3">
+        <f>C22/D22</f>
+        <v>0.10234713384325206</v>
+      </c>
+      <c r="F22" s="4">
+        <f t="shared" ref="F22:F26" si="3">F21+C21+$O$2</f>
+        <v>147.35990620944301</v>
+      </c>
+      <c r="G22" s="3">
+        <f>F22/D22</f>
+        <v>0.34269745630103027</v>
+      </c>
+      <c r="H22" s="5">
+        <v>4</v>
+      </c>
+      <c r="I22" s="7">
+        <f t="shared" si="0"/>
+        <v>0.58724782252661356</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -1329,29 +1395,30 @@
       <c r="B23" t="s">
         <v>55</v>
       </c>
-      <c r="C23">
-        <v>58.564999999999998</v>
+      <c r="C23" s="4">
+        <v>47.509728188348838</v>
       </c>
       <c r="D23" s="1">
         <v>430</v>
       </c>
-      <c r="E23" s="4">
-        <v>3.9689999999999999</v>
-      </c>
-      <c r="F23" s="3">
-        <f t="shared" si="0"/>
-        <v>0.13619767441860464</v>
-      </c>
-      <c r="G23" s="4">
+      <c r="E23" s="3">
+        <f>C23/D23</f>
+        <v>0.11048773997290427</v>
+      </c>
+      <c r="F23" s="4">
         <f t="shared" si="3"/>
-        <v>187.99299999999999</v>
-      </c>
-      <c r="H23" s="3">
-        <f t="shared" si="1"/>
-        <v>0.43719302325581394</v>
-      </c>
-      <c r="I23">
-        <v>0.55000000000000004</v>
+        <v>195.33817376204138</v>
+      </c>
+      <c r="G23" s="3">
+        <f>F23/D23</f>
+        <v>0.45427482270242181</v>
+      </c>
+      <c r="H23" s="5">
+        <v>4</v>
+      </c>
+      <c r="I23" s="7">
+        <f t="shared" si="0"/>
+        <v>0.58724782252661356</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
@@ -1361,29 +1428,30 @@
       <c r="B24" t="s">
         <v>56</v>
       </c>
-      <c r="C24">
-        <v>57.49</v>
+      <c r="C24" s="4">
+        <v>46.637655144679847</v>
       </c>
       <c r="D24" s="1">
         <v>430</v>
       </c>
-      <c r="E24" s="4">
-        <v>3.9689999999999999</v>
-      </c>
-      <c r="F24" s="3">
-        <f t="shared" si="0"/>
-        <v>0.13369767441860467</v>
-      </c>
-      <c r="G24" s="4">
+      <c r="E24" s="3">
+        <f>C24/D24</f>
+        <v>0.10845966312716243</v>
+      </c>
+      <c r="F24" s="4">
         <f t="shared" si="3"/>
-        <v>250.52699999999999</v>
-      </c>
-      <c r="H24" s="3">
-        <f t="shared" si="1"/>
-        <v>0.58262093023255812</v>
-      </c>
-      <c r="I24">
-        <v>0.55000000000000004</v>
+        <v>246.81690195039022</v>
+      </c>
+      <c r="G24" s="3">
+        <f>F24/D24</f>
+        <v>0.57399279523346558</v>
+      </c>
+      <c r="H24" s="5">
+        <v>4</v>
+      </c>
+      <c r="I24" s="7">
+        <f t="shared" si="0"/>
+        <v>0.58724782252661356</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
@@ -1393,29 +1461,30 @@
       <c r="B25" t="s">
         <v>57</v>
       </c>
-      <c r="C25">
-        <v>45.6</v>
+      <c r="C25" s="4">
+        <v>36.992121666331549</v>
       </c>
       <c r="D25" s="1">
         <v>430</v>
       </c>
-      <c r="E25" s="4">
-        <v>3.9689999999999999</v>
-      </c>
-      <c r="F25" s="3">
-        <f t="shared" si="0"/>
-        <v>0.10604651162790699</v>
-      </c>
-      <c r="G25" s="4">
+      <c r="E25" s="3">
+        <f>C25/D25</f>
+        <v>8.6028189921701276E-2</v>
+      </c>
+      <c r="F25" s="4">
         <f t="shared" si="3"/>
-        <v>311.98599999999999</v>
-      </c>
-      <c r="H25" s="3">
-        <f t="shared" si="1"/>
-        <v>0.7255488372093023</v>
-      </c>
-      <c r="I25">
-        <v>0.55000000000000004</v>
+        <v>297.42355709507007</v>
+      </c>
+      <c r="G25" s="3">
+        <f>F25/D25</f>
+        <v>0.69168269091876755</v>
+      </c>
+      <c r="H25" s="5">
+        <v>4</v>
+      </c>
+      <c r="I25" s="7">
+        <f t="shared" si="0"/>
+        <v>0.58724782252661356</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -1425,38 +1494,42 @@
       <c r="B26" t="s">
         <v>58</v>
       </c>
-      <c r="C26">
-        <v>44.277000000000001</v>
+      <c r="C26" s="4">
+        <v>35.918863399564955</v>
       </c>
       <c r="D26" s="1">
         <v>430</v>
       </c>
-      <c r="E26" s="4">
-        <v>3.9689999999999999</v>
-      </c>
-      <c r="F26" s="3">
-        <f t="shared" si="0"/>
-        <v>0.10296976744186047</v>
-      </c>
-      <c r="G26" s="4">
+      <c r="E26" s="3">
+        <f>C26/D26</f>
+        <v>8.3532240464104554E-2</v>
+      </c>
+      <c r="F26" s="4">
         <f t="shared" si="3"/>
-        <v>361.55500000000001</v>
-      </c>
-      <c r="H26" s="3">
-        <f t="shared" si="1"/>
-        <v>0.8408255813953488</v>
-      </c>
-      <c r="I26">
-        <v>0.55000000000000004</v>
+        <v>338.38467876140163</v>
+      </c>
+      <c r="G26" s="3">
+        <f>F26/D26</f>
+        <v>0.78694111339860839</v>
+      </c>
+      <c r="H26" s="5">
+        <v>4</v>
+      </c>
+      <c r="I26" s="7">
+        <f t="shared" si="0"/>
+        <v>0.58724782252661356</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="A30" s="8" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A30" r:id="rId1" xr:uid="{E95C198A-033F-40E6-B108-FDCD04F54A60}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>